<commit_message>
update file with jgit
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Repository.TestGitCommitChangesOutsideWebstudio/Main.xlsx
+++ b/DESIGN/rules/Repository.TestGitCommitChangesOutsideWebstudio/Main.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
@@ -224,9 +224,6 @@
     <t>R10</t>
   </si>
   <si>
-    <t>Good Morning</t>
-  </si>
-  <si>
     <t>R20</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
+  </si>
+  <si>
+    <t>GIT UPDATE</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -981,7 +983,7 @@
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -998,7 +1000,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -1010,16 +1012,16 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>5</v>
@@ -1050,12 +1052,12 @@
         <v>11</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="20">
         <v>12</v>
@@ -1064,12 +1066,12 @@
         <v>17</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="20">
         <v>18</v>
@@ -1078,12 +1080,12 @@
         <v>21</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>
@@ -1092,7 +1094,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>